<commit_message>
Sample file for trend analysis
</commit_message>
<xml_diff>
--- a/WEG_Billing_2025-08.xlsx
+++ b/WEG_Billing_2025-08.xlsx
@@ -3,16 +3,14 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <workbookPr codeName="ThisWorkbook"/>
   <sheets>
-    <sheet name="2025-05" sheetId="1" r:id="rId1"/>
-    <sheet name="2025-06" sheetId="2" r:id="rId2"/>
-    <sheet name="2025-07" sheetId="3" r:id="rId3"/>
-    <sheet name="2025-08" sheetId="4" r:id="rId4"/>
+    <sheet name="2025-06" sheetId="1" r:id="rId1"/>
+    <sheet name="2025-07" sheetId="2" r:id="rId2"/>
+    <sheet name="2025-08" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0">'2025-05'!$A$4:$E$51</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1">'2025-06'!$A$4:$E$51</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2">'2025-07'!$A$4:$E$51</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3">'2025-08'!$A$4:$E$51</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0">'2025-06'!$A$4:$E$51</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1">'2025-07'!$A$4:$E$51</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2">'2025-08'!$A$4:$E$51</definedName>
   </definedNames>
 </workbook>
 </file>
@@ -436,7 +434,7 @@
         <v>WEG Billing – Month</v>
       </c>
       <c r="B1" s="1" t="str">
-        <v>2025-05</v>
+        <v>2025-06</v>
       </c>
     </row>
     <row r="2">
@@ -444,7 +442,7 @@
         <v>Generated at</v>
       </c>
       <c r="B2" t="str">
-        <v>8/31/2025, 8:55:48 AM</v>
+        <v>9/1/2025, 10:29:50 AM</v>
       </c>
     </row>
     <row r="4">
@@ -472,7 +470,7 @@
         <v>A4</v>
       </c>
       <c r="D5" s="2">
-        <v>1000</v>
+        <v>1458575</v>
       </c>
       <c r="E5" t="str">
         <v>kWh</v>
@@ -489,7 +487,7 @@
         <v>B4</v>
       </c>
       <c r="D6" s="3">
-        <v>5000</v>
+        <v>880925</v>
       </c>
       <c r="E6" t="str">
         <v>₹</v>
@@ -506,7 +504,7 @@
         <v>C4</v>
       </c>
       <c r="D7" s="3">
-        <v>8000</v>
+        <v>6126015</v>
       </c>
       <c r="E7" t="str">
         <v>₹</v>
@@ -523,7 +521,7 @@
         <v>D4</v>
       </c>
       <c r="D8" s="3">
-        <v>200</v>
+        <v>0</v>
       </c>
       <c r="E8" t="str">
         <v>₹</v>
@@ -540,7 +538,7 @@
         <v>E4</v>
       </c>
       <c r="D9" s="3">
-        <v>300</v>
+        <v>3573508.75</v>
       </c>
       <c r="E9" t="str">
         <v>₹</v>
@@ -557,7 +555,7 @@
         <v>F4</v>
       </c>
       <c r="D10" s="3">
-        <v>100</v>
+        <v>143961.35</v>
       </c>
       <c r="E10" t="str">
         <v>₹</v>
@@ -574,7 +572,7 @@
         <v>G4</v>
       </c>
       <c r="D11" s="3">
-        <v>50</v>
+        <v>91890.23</v>
       </c>
       <c r="E11" t="str">
         <v>₹</v>
@@ -591,7 +589,7 @@
         <v>H4</v>
       </c>
       <c r="D12" s="3">
-        <v>400</v>
+        <v>414268.75</v>
       </c>
       <c r="E12" t="str">
         <v>₹</v>
@@ -608,7 +606,7 @@
         <v>I4</v>
       </c>
       <c r="D13" s="3">
-        <v>600</v>
+        <v>0</v>
       </c>
       <c r="E13" t="str">
         <v>₹</v>
@@ -625,7 +623,7 @@
         <v>A9</v>
       </c>
       <c r="D14" s="3">
-        <v>14350</v>
+        <v>10758865.92</v>
       </c>
       <c r="E14" t="str">
         <v>₹</v>
@@ -642,7 +640,7 @@
         <v>B9</v>
       </c>
       <c r="D15" s="3">
-        <v>2870</v>
+        <v>2151773.184</v>
       </c>
       <c r="E15" t="str">
         <v>₹</v>
@@ -659,7 +657,7 @@
         <v>C9</v>
       </c>
       <c r="D16" s="3">
-        <v>17220</v>
+        <v>12910639.104</v>
       </c>
       <c r="E16" t="str">
         <v>₹</v>
@@ -676,7 +674,7 @@
         <v>D9</v>
       </c>
       <c r="D18" s="3">
-        <v>200</v>
+        <v>16232571.78</v>
       </c>
       <c r="E18" t="str">
         <v>₹</v>
@@ -693,7 +691,7 @@
         <v>E9</v>
       </c>
       <c r="D19" s="3">
-        <v>50</v>
+        <v>16222328.84</v>
       </c>
       <c r="E19" t="str">
         <v>₹</v>
@@ -710,7 +708,7 @@
         <v>F9</v>
       </c>
       <c r="D20" s="3">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="E20" t="str">
         <v>₹</v>
@@ -727,7 +725,7 @@
         <v>G9</v>
       </c>
       <c r="D21" s="3">
-        <v>0</v>
+        <v>5274956.17</v>
       </c>
       <c r="E21" t="str">
         <v>₹</v>
@@ -744,7 +742,7 @@
         <v>H9</v>
       </c>
       <c r="D22" s="3">
-        <v>17450</v>
+        <v>23868254.714</v>
       </c>
       <c r="E22" t="str">
         <v>₹</v>
@@ -761,7 +759,7 @@
         <v>I9</v>
       </c>
       <c r="D23" s="3">
-        <v>17400</v>
+        <v>7645925.874000002</v>
       </c>
       <c r="E23" t="str">
         <v>₹</v>
@@ -778,7 +776,7 @@
         <v>A31</v>
       </c>
       <c r="D24" s="3">
-        <v>150</v>
+        <v>10242.939999999478</v>
       </c>
       <c r="E24" t="str">
         <v>₹</v>
@@ -795,7 +793,7 @@
         <v>B15</v>
       </c>
       <c r="D26" s="4">
-        <v>0.3</v>
+        <v>0.32</v>
       </c>
       <c r="E26" t="str">
         <v>%</v>
@@ -812,7 +810,7 @@
         <v>D15</v>
       </c>
       <c r="D27" s="4">
-        <v>0.7</v>
+        <v>0.21</v>
       </c>
       <c r="E27" t="str">
         <v>%</v>
@@ -829,7 +827,7 @@
         <v>C16</v>
       </c>
       <c r="D28" s="4">
-        <v>0.02</v>
+        <v>0.0362</v>
       </c>
       <c r="E28" t="str">
         <v>%</v>
@@ -846,7 +844,7 @@
         <v>A17</v>
       </c>
       <c r="D29" s="5">
-        <v>1</v>
+        <v>520.279</v>
       </c>
       <c r="E29" t="str">
         <v>MWh</v>
@@ -863,7 +861,7 @@
         <v>B17</v>
       </c>
       <c r="D30" s="5">
-        <v>1</v>
+        <v>268.022</v>
       </c>
       <c r="E30" t="str">
         <v>MWh</v>
@@ -880,7 +878,7 @@
         <v>C17</v>
       </c>
       <c r="D31" s="5">
-        <v>2</v>
+        <v>276.496</v>
       </c>
       <c r="E31" t="str">
         <v>MWh</v>
@@ -897,7 +895,7 @@
         <v>D17</v>
       </c>
       <c r="D32" s="5">
-        <v>1</v>
+        <v>685.229</v>
       </c>
       <c r="E32" t="str">
         <v>MWh</v>
@@ -914,7 +912,7 @@
         <v>E17</v>
       </c>
       <c r="D33" s="5">
-        <v>1</v>
+        <v>240.431</v>
       </c>
       <c r="E33" t="str">
         <v>MWh</v>
@@ -931,7 +929,7 @@
         <v>A18</v>
       </c>
       <c r="D34" s="2">
-        <v>588</v>
+        <v>243125</v>
       </c>
       <c r="E34" t="str">
         <v>kWh</v>
@@ -948,7 +946,7 @@
         <v>C18</v>
       </c>
       <c r="D35" s="2">
-        <v>2744</v>
+        <v>243314</v>
       </c>
       <c r="E35" t="str">
         <v>kWh</v>
@@ -965,7 +963,7 @@
         <v>A19</v>
       </c>
       <c r="D36" s="2">
-        <v>3332</v>
+        <v>486439</v>
       </c>
       <c r="E36" t="str">
         <v>kWh</v>
@@ -982,7 +980,7 @@
         <v>A24</v>
       </c>
       <c r="D38" s="3">
-        <v>500</v>
+        <v>3381394.62</v>
       </c>
       <c r="E38" t="str">
         <v>₹</v>
@@ -999,7 +997,7 @@
         <v>B24</v>
       </c>
       <c r="D39" s="3">
-        <v>200</v>
+        <v>676278.93</v>
       </c>
       <c r="E39" t="str">
         <v>₹</v>
@@ -1016,7 +1014,7 @@
         <v>C24</v>
       </c>
       <c r="D40" s="3">
-        <v>100</v>
+        <v>1274756.85</v>
       </c>
       <c r="E40" t="str">
         <v>₹</v>
@@ -1033,7 +1031,7 @@
         <v>D24</v>
       </c>
       <c r="D41" s="3">
-        <v>50</v>
+        <v>26865.65</v>
       </c>
       <c r="E41" t="str">
         <v>₹</v>
@@ -1050,7 +1048,7 @@
         <v>E24</v>
       </c>
       <c r="D42" s="3">
-        <v>25</v>
+        <v>5373.13</v>
       </c>
       <c r="E42" t="str">
         <v>₹</v>
@@ -1067,7 +1065,7 @@
         <v>F24</v>
       </c>
       <c r="D43" s="3">
-        <v>25</v>
+        <v>25235.45</v>
       </c>
       <c r="E43" t="str">
         <v>₹</v>
@@ -1084,7 +1082,7 @@
         <v>A26</v>
       </c>
       <c r="D44" s="3">
-        <v>700</v>
+        <v>4057673.5500000003</v>
       </c>
       <c r="E44" t="str">
         <v>₹</v>
@@ -1101,7 +1099,7 @@
         <v>B26</v>
       </c>
       <c r="D45" s="3">
-        <v>100</v>
+        <v>57474.23</v>
       </c>
       <c r="E45" t="str">
         <v>₹</v>
@@ -1118,7 +1116,7 @@
         <v>C26</v>
       </c>
       <c r="D46" s="3">
-        <v>600</v>
+        <v>4000199.3200000003</v>
       </c>
       <c r="E46" t="str">
         <v>₹</v>
@@ -1135,7 +1133,7 @@
         <v>B19</v>
       </c>
       <c r="D47" s="6">
-        <v>0.18007202881152462</v>
+        <v>8.223434634147345</v>
       </c>
       <c r="E47" t="str">
         <v>₹/kWh</v>
@@ -1152,7 +1150,7 @@
         <v>F16</v>
       </c>
       <c r="D48" s="3">
-        <v>105.88235294117648</v>
+        <v>1999322.5454270733</v>
       </c>
       <c r="E48" t="str">
         <v>₹</v>
@@ -1169,7 +1167,7 @@
         <v>G16</v>
       </c>
       <c r="D49" s="3">
-        <v>494.11764705882354</v>
+        <v>2000876.7745729273</v>
       </c>
       <c r="E49" t="str">
         <v>₹</v>
@@ -1186,7 +1184,7 @@
         <v>—</v>
       </c>
       <c r="D51" s="3">
-        <v>16700</v>
+        <v>7645925.874</v>
       </c>
       <c r="E51" t="str">
         <v>₹</v>
@@ -1235,7 +1233,7 @@
         <v>0</v>
       </c>
       <c r="F54" s="7">
-        <v>750</v>
+        <v>0</v>
       </c>
       <c r="G54" s="7">
         <v>0</v>
@@ -1304,22 +1302,22 @@
         <v>MD Slab 3</v>
       </c>
       <c r="C57" s="7">
-        <v>-421.05</v>
+        <v>1423</v>
       </c>
       <c r="D57" s="7">
         <v>475</v>
       </c>
       <c r="E57" s="7">
-        <v>-199998.75</v>
+        <v>675925</v>
       </c>
       <c r="F57" s="7">
         <v>475</v>
       </c>
       <c r="G57" s="7">
-        <v>-421.05</v>
+        <v>1423</v>
       </c>
       <c r="H57" s="7">
-        <v>-199998.75</v>
+        <v>675925</v>
       </c>
     </row>
     <row r="58">
@@ -1339,7 +1337,7 @@
         <v>0</v>
       </c>
       <c r="F58" s="7">
-        <v>370</v>
+        <v>0</v>
       </c>
       <c r="G58" s="7">
         <v>0</v>
@@ -1356,22 +1354,22 @@
         <v>Energy Charge Slab 1</v>
       </c>
       <c r="C59" s="7">
-        <v>1000</v>
+        <v>1458575</v>
       </c>
       <c r="D59" s="7">
         <v>4.2</v>
       </c>
       <c r="E59" s="7">
-        <v>4200</v>
+        <v>6126015</v>
       </c>
       <c r="F59" s="7">
         <v>4.2</v>
       </c>
       <c r="G59" s="7">
-        <v>1000</v>
+        <v>1458575</v>
       </c>
       <c r="H59" s="7">
-        <v>4200</v>
+        <v>6126015</v>
       </c>
     </row>
     <row r="60">
@@ -1382,22 +1380,22 @@
         <v>FCA</v>
       </c>
       <c r="C60" s="7">
-        <v>1000</v>
+        <v>1458575</v>
       </c>
       <c r="D60" s="7">
         <v>2.45</v>
       </c>
       <c r="E60" s="7">
-        <v>2450</v>
+        <v>3573508.7500000005</v>
       </c>
       <c r="F60" s="7">
         <v>1.81</v>
       </c>
       <c r="G60" s="7">
-        <v>1353.5911602209944</v>
+        <v>1974314.2265193372</v>
       </c>
       <c r="H60" s="7">
-        <v>2450</v>
+        <v>3573508.7500000005</v>
       </c>
     </row>
     <row r="61">
@@ -1408,22 +1406,22 @@
         <v>TOD Peak</v>
       </c>
       <c r="C61" s="7">
-        <v>470.59</v>
+        <v>487375</v>
       </c>
       <c r="D61" s="7">
         <v>0.85</v>
       </c>
       <c r="E61" s="7">
-        <v>400.00149999999996</v>
+        <v>414268.75</v>
       </c>
       <c r="F61" s="7">
         <v>0.85</v>
       </c>
       <c r="G61" s="7">
-        <v>470.59</v>
+        <v>487375</v>
       </c>
       <c r="H61" s="7">
-        <v>400.00149999999996</v>
+        <v>414268.75</v>
       </c>
     </row>
     <row r="62">
@@ -1434,22 +1432,22 @@
         <v>TOD Night Rebate</v>
       </c>
       <c r="C62" s="7">
-        <v>-33.33</v>
+        <v>-6126015.33</v>
       </c>
       <c r="D62" s="7">
-        <v>1.5</v>
+        <v>0.015</v>
       </c>
       <c r="E62" s="7">
-        <v>-49.995</v>
+        <v>-91890.22995</v>
       </c>
       <c r="F62" s="7">
         <v>0.43</v>
       </c>
       <c r="G62" s="7">
-        <v>-116.26744186046511</v>
+        <v>-213698.2091860465</v>
       </c>
       <c r="H62" s="7">
-        <v>-49.995</v>
+        <v>-91890.22995</v>
       </c>
     </row>
     <row r="63">
@@ -1460,22 +1458,22 @@
         <v>PF Charge Slab 1</v>
       </c>
       <c r="C63" s="7">
-        <v>-33.33</v>
+        <v>-6126015.33</v>
       </c>
       <c r="D63" s="7">
-        <v>2.35</v>
+        <v>0.0235</v>
       </c>
       <c r="E63" s="7">
-        <v>-78.3255</v>
+        <v>-143961.360255</v>
       </c>
       <c r="F63" s="7">
         <v>0.02</v>
       </c>
       <c r="G63" s="7">
-        <v>-3916.275</v>
+        <v>-7198068.01275</v>
       </c>
       <c r="H63" s="7">
-        <v>-78.3255</v>
+        <v>-143961.360255</v>
       </c>
     </row>
     <row r="64">
@@ -1489,13 +1487,13 @@
         <v>0</v>
       </c>
       <c r="D64" s="7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E64" s="7">
         <v>0</v>
       </c>
       <c r="F64" s="7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G64" s="7">
         <v>0</v>
@@ -1512,22 +1510,22 @@
         <v>Arrear ED</v>
       </c>
       <c r="C65" s="7">
-        <v>14350</v>
+        <v>10758865.92</v>
       </c>
       <c r="D65" s="7">
         <v>0.2</v>
       </c>
       <c r="E65" s="7">
-        <v>2870</v>
+        <v>2151773.184</v>
       </c>
       <c r="F65" s="7">
         <v>1</v>
       </c>
       <c r="G65" s="7">
-        <v>2870</v>
+        <v>2151773.184</v>
       </c>
       <c r="H65" s="7">
-        <v>2870</v>
+        <v>2151773.184</v>
       </c>
     </row>
     <row r="66">
@@ -1541,13 +1539,13 @@
         <v>0</v>
       </c>
       <c r="D66" s="7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E66" s="7">
         <v>0</v>
       </c>
       <c r="F66" s="7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G66" s="7">
         <v>0</v>
@@ -1567,13 +1565,13 @@
         <v>0</v>
       </c>
       <c r="D67" s="7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E67" s="7">
         <v>0</v>
       </c>
       <c r="F67" s="7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G67" s="7">
         <v>0</v>
@@ -1593,13 +1591,13 @@
         <v>0</v>
       </c>
       <c r="D68" s="7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E68" s="7">
         <v>0</v>
       </c>
       <c r="F68" s="7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G68" s="7">
         <v>0</v>
@@ -1625,7 +1623,7 @@
         <v>0</v>
       </c>
       <c r="F69" s="7">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="G69" s="7">
         <v>0</v>
@@ -1664,7 +1662,7 @@
         <v>WEG Billing – Month</v>
       </c>
       <c r="B1" s="1" t="str">
-        <v>2025-06</v>
+        <v>2025-07</v>
       </c>
     </row>
     <row r="2">
@@ -1672,7 +1670,7 @@
         <v>Generated at</v>
       </c>
       <c r="B2" t="str">
-        <v>8/31/2025, 8:55:52 AM</v>
+        <v>9/1/2025, 10:16:31 AM</v>
       </c>
     </row>
     <row r="4">
@@ -1700,7 +1698,7 @@
         <v>A4</v>
       </c>
       <c r="D5" s="2">
-        <v>1000</v>
+        <v>1483312.5</v>
       </c>
       <c r="E5" t="str">
         <v>kWh</v>
@@ -1717,7 +1715,7 @@
         <v>B4</v>
       </c>
       <c r="D6" s="3">
-        <v>5000</v>
+        <v>880925</v>
       </c>
       <c r="E6" t="str">
         <v>₹</v>
@@ -1734,7 +1732,7 @@
         <v>C4</v>
       </c>
       <c r="D7" s="3">
-        <v>8000</v>
+        <v>6229914.6</v>
       </c>
       <c r="E7" t="str">
         <v>₹</v>
@@ -1751,7 +1749,7 @@
         <v>D4</v>
       </c>
       <c r="D8" s="3">
-        <v>200</v>
+        <v>0</v>
       </c>
       <c r="E8" t="str">
         <v>₹</v>
@@ -1768,7 +1766,7 @@
         <v>E4</v>
       </c>
       <c r="D9" s="3">
-        <v>300</v>
+        <v>3634116.85</v>
       </c>
       <c r="E9" t="str">
         <v>₹</v>
@@ -1785,7 +1783,7 @@
         <v>F4</v>
       </c>
       <c r="D10" s="3">
-        <v>100</v>
+        <v>146402.99</v>
       </c>
       <c r="E10" t="str">
         <v>₹</v>
@@ -1802,7 +1800,7 @@
         <v>G4</v>
       </c>
       <c r="D11" s="3">
-        <v>50</v>
+        <v>93448.72</v>
       </c>
       <c r="E11" t="str">
         <v>₹</v>
@@ -1819,7 +1817,7 @@
         <v>H4</v>
       </c>
       <c r="D12" s="3">
-        <v>400</v>
+        <v>418954.8</v>
       </c>
       <c r="E12" t="str">
         <v>₹</v>
@@ -1836,7 +1834,7 @@
         <v>I4</v>
       </c>
       <c r="D13" s="3">
-        <v>600</v>
+        <v>0</v>
       </c>
       <c r="E13" t="str">
         <v>₹</v>
@@ -1853,7 +1851,7 @@
         <v>A9</v>
       </c>
       <c r="D14" s="3">
-        <v>14350</v>
+        <v>10924059.54</v>
       </c>
       <c r="E14" t="str">
         <v>₹</v>
@@ -1870,7 +1868,7 @@
         <v>B9</v>
       </c>
       <c r="D15" s="3">
-        <v>2870</v>
+        <v>2184811.908</v>
       </c>
       <c r="E15" t="str">
         <v>₹</v>
@@ -1887,7 +1885,7 @@
         <v>C9</v>
       </c>
       <c r="D16" s="3">
-        <v>17220</v>
+        <v>13108871.447999999</v>
       </c>
       <c r="E16" t="str">
         <v>₹</v>
@@ -1904,7 +1902,7 @@
         <v>D9</v>
       </c>
       <c r="D18" s="3">
-        <v>200</v>
+        <v>16227158.84</v>
       </c>
       <c r="E18" t="str">
         <v>₹</v>
@@ -1921,7 +1919,7 @@
         <v>E9</v>
       </c>
       <c r="D19" s="3">
-        <v>50</v>
+        <v>16222328.84</v>
       </c>
       <c r="E19" t="str">
         <v>₹</v>
@@ -1938,7 +1936,7 @@
         <v>F9</v>
       </c>
       <c r="D20" s="3">
-        <v>30</v>
+        <v>25.98</v>
       </c>
       <c r="E20" t="str">
         <v>₹</v>
@@ -1955,7 +1953,7 @@
         <v>G9</v>
       </c>
       <c r="D21" s="3">
-        <v>0</v>
+        <v>6456080.43</v>
       </c>
       <c r="E21" t="str">
         <v>₹</v>
@@ -1972,7 +1970,7 @@
         <v>H9</v>
       </c>
       <c r="D22" s="3">
-        <v>17450</v>
+        <v>22879975.838</v>
       </c>
       <c r="E22" t="str">
         <v>₹</v>
@@ -1989,7 +1987,7 @@
         <v>I9</v>
       </c>
       <c r="D23" s="3">
-        <v>17400</v>
+        <v>6657646.998</v>
       </c>
       <c r="E23" t="str">
         <v>₹</v>
@@ -2006,7 +2004,7 @@
         <v>A31</v>
       </c>
       <c r="D24" s="3">
-        <v>150</v>
+        <v>4830</v>
       </c>
       <c r="E24" t="str">
         <v>₹</v>
@@ -2023,7 +2021,7 @@
         <v>B15</v>
       </c>
       <c r="D26" s="4">
-        <v>0.3</v>
+        <v>0.32</v>
       </c>
       <c r="E26" t="str">
         <v>%</v>
@@ -2040,7 +2038,7 @@
         <v>D15</v>
       </c>
       <c r="D27" s="4">
-        <v>0.7</v>
+        <v>0.21</v>
       </c>
       <c r="E27" t="str">
         <v>%</v>
@@ -2057,7 +2055,7 @@
         <v>C16</v>
       </c>
       <c r="D28" s="4">
-        <v>0.02</v>
+        <v>0.036699999999999997</v>
       </c>
       <c r="E28" t="str">
         <v>%</v>
@@ -2074,7 +2072,7 @@
         <v>A17</v>
       </c>
       <c r="D29" s="5">
-        <v>1</v>
+        <v>589.802</v>
       </c>
       <c r="E29" t="str">
         <v>MWh</v>
@@ -2091,7 +2089,7 @@
         <v>B17</v>
       </c>
       <c r="D30" s="5">
-        <v>1</v>
+        <v>303.838</v>
       </c>
       <c r="E30" t="str">
         <v>MWh</v>
@@ -2108,7 +2106,7 @@
         <v>C17</v>
       </c>
       <c r="D31" s="5">
-        <v>2</v>
+        <v>593.458</v>
       </c>
       <c r="E31" t="str">
         <v>MWh</v>
@@ -2125,7 +2123,7 @@
         <v>D17</v>
       </c>
       <c r="D32" s="5">
-        <v>1</v>
+        <v>1470.745</v>
       </c>
       <c r="E32" t="str">
         <v>MWh</v>
@@ -2142,7 +2140,7 @@
         <v>E17</v>
       </c>
       <c r="D33" s="5">
-        <v>1</v>
+        <v>516.051</v>
       </c>
       <c r="E33" t="str">
         <v>MWh</v>
@@ -2159,7 +2157,7 @@
         <v>A18</v>
       </c>
       <c r="D34" s="2">
-        <v>588</v>
+        <v>275470</v>
       </c>
       <c r="E34" t="str">
         <v>kWh</v>
@@ -2176,7 +2174,7 @@
         <v>C18</v>
       </c>
       <c r="D35" s="2">
-        <v>2744</v>
+        <v>521968</v>
       </c>
       <c r="E35" t="str">
         <v>kWh</v>
@@ -2193,7 +2191,7 @@
         <v>A19</v>
       </c>
       <c r="D36" s="2">
-        <v>3332</v>
+        <v>797438</v>
       </c>
       <c r="E36" t="str">
         <v>kWh</v>
@@ -2210,7 +2208,7 @@
         <v>A24</v>
       </c>
       <c r="D38" s="3">
-        <v>500</v>
+        <v>5415447.6</v>
       </c>
       <c r="E38" t="str">
         <v>₹</v>
@@ -2227,7 +2225,7 @@
         <v>B24</v>
       </c>
       <c r="D39" s="3">
-        <v>200</v>
+        <v>1083089.52</v>
       </c>
       <c r="E39" t="str">
         <v>₹</v>
@@ -2244,7 +2242,7 @@
         <v>C24</v>
       </c>
       <c r="D40" s="3">
-        <v>100</v>
+        <v>8150</v>
       </c>
       <c r="E40" t="str">
         <v>₹</v>
@@ -2261,7 +2259,7 @@
         <v>D24</v>
       </c>
       <c r="D41" s="3">
-        <v>50</v>
+        <v>7679.81</v>
       </c>
       <c r="E41" t="str">
         <v>₹</v>
@@ -2278,7 +2276,7 @@
         <v>E24</v>
       </c>
       <c r="D42" s="3">
-        <v>25</v>
+        <v>1535.97</v>
       </c>
       <c r="E42" t="str">
         <v>₹</v>
@@ -2295,7 +2293,7 @@
         <v>F24</v>
       </c>
       <c r="D43" s="3">
-        <v>25</v>
+        <v>41390.91</v>
       </c>
       <c r="E43" t="str">
         <v>₹</v>
@@ -2312,7 +2310,7 @@
         <v>A26</v>
       </c>
       <c r="D44" s="3">
-        <v>700</v>
+        <v>6498537.119999999</v>
       </c>
       <c r="E44" t="str">
         <v>₹</v>
@@ -2329,7 +2327,7 @@
         <v>B26</v>
       </c>
       <c r="D45" s="3">
-        <v>100</v>
+        <v>50606.69</v>
       </c>
       <c r="E45" t="str">
         <v>₹</v>
@@ -2346,7 +2344,7 @@
         <v>C26</v>
       </c>
       <c r="D46" s="3">
-        <v>600</v>
+        <v>6447930.429999999</v>
       </c>
       <c r="E46" t="str">
         <v>₹</v>
@@ -2363,7 +2361,7 @@
         <v>B19</v>
       </c>
       <c r="D47" s="6">
-        <v>0.18007202881152462</v>
+        <v>8.085807837098306</v>
       </c>
       <c r="E47" t="str">
         <v>₹/kWh</v>
@@ -2380,7 +2378,7 @@
         <v>F16</v>
       </c>
       <c r="D48" s="3">
-        <v>105.88235294117648</v>
+        <v>2227397.4848854705</v>
       </c>
       <c r="E48" t="str">
         <v>₹</v>
@@ -2397,7 +2395,7 @@
         <v>G16</v>
       </c>
       <c r="D49" s="3">
-        <v>494.11764705882354</v>
+        <v>4220532.945114529</v>
       </c>
       <c r="E49" t="str">
         <v>₹</v>
@@ -2414,7 +2412,7 @@
         <v>—</v>
       </c>
       <c r="D51" s="3">
-        <v>16700</v>
+        <v>6657646.998</v>
       </c>
       <c r="E51" t="str">
         <v>₹</v>
@@ -2463,7 +2461,7 @@
         <v>0</v>
       </c>
       <c r="F54" s="7">
-        <v>750</v>
+        <v>0</v>
       </c>
       <c r="G54" s="7">
         <v>0</v>
@@ -2532,22 +2530,22 @@
         <v>MD Slab 3</v>
       </c>
       <c r="C57" s="7">
-        <v>-421.05</v>
+        <v>1423</v>
       </c>
       <c r="D57" s="7">
         <v>475</v>
       </c>
       <c r="E57" s="7">
-        <v>-199998.75</v>
+        <v>675925</v>
       </c>
       <c r="F57" s="7">
         <v>475</v>
       </c>
       <c r="G57" s="7">
-        <v>-421.05</v>
+        <v>1423</v>
       </c>
       <c r="H57" s="7">
-        <v>-199998.75</v>
+        <v>675925</v>
       </c>
     </row>
     <row r="58">
@@ -2567,7 +2565,7 @@
         <v>0</v>
       </c>
       <c r="F58" s="7">
-        <v>370</v>
+        <v>0</v>
       </c>
       <c r="G58" s="7">
         <v>0</v>
@@ -2584,22 +2582,22 @@
         <v>Energy Charge Slab 1</v>
       </c>
       <c r="C59" s="7">
-        <v>1000</v>
+        <v>1483312.5</v>
       </c>
       <c r="D59" s="7">
         <v>4.2</v>
       </c>
       <c r="E59" s="7">
-        <v>4200</v>
+        <v>6229912.5</v>
       </c>
       <c r="F59" s="7">
         <v>4.2</v>
       </c>
       <c r="G59" s="7">
-        <v>1000</v>
+        <v>1483312.5</v>
       </c>
       <c r="H59" s="7">
-        <v>4200</v>
+        <v>6229912.5</v>
       </c>
     </row>
     <row r="60">
@@ -2610,22 +2608,22 @@
         <v>FCA</v>
       </c>
       <c r="C60" s="7">
-        <v>1000</v>
+        <v>1483312.5</v>
       </c>
       <c r="D60" s="7">
         <v>2.45</v>
       </c>
       <c r="E60" s="7">
-        <v>2450</v>
+        <v>3634115.6250000005</v>
       </c>
       <c r="F60" s="7">
         <v>1.81</v>
       </c>
       <c r="G60" s="7">
-        <v>1353.5911602209944</v>
+        <v>2007798.6878453041</v>
       </c>
       <c r="H60" s="7">
-        <v>2450</v>
+        <v>3634115.6250000005</v>
       </c>
     </row>
     <row r="61">
@@ -2636,22 +2634,22 @@
         <v>TOD Peak</v>
       </c>
       <c r="C61" s="7">
-        <v>470.59</v>
+        <v>492888</v>
       </c>
       <c r="D61" s="7">
         <v>0.85</v>
       </c>
       <c r="E61" s="7">
-        <v>400.00149999999996</v>
+        <v>418954.8</v>
       </c>
       <c r="F61" s="7">
         <v>0.85</v>
       </c>
       <c r="G61" s="7">
-        <v>470.59</v>
+        <v>492888</v>
       </c>
       <c r="H61" s="7">
-        <v>400.00149999999996</v>
+        <v>418954.8</v>
       </c>
     </row>
     <row r="62">
@@ -2662,22 +2660,22 @@
         <v>TOD Night Rebate</v>
       </c>
       <c r="C62" s="7">
-        <v>-33.33</v>
+        <v>-6229914.67</v>
       </c>
       <c r="D62" s="7">
-        <v>1.5</v>
+        <v>0.015</v>
       </c>
       <c r="E62" s="7">
-        <v>-49.995</v>
+        <v>-93448.72004999999</v>
       </c>
       <c r="F62" s="7">
         <v>0.43</v>
       </c>
       <c r="G62" s="7">
-        <v>-116.26744186046511</v>
+        <v>-217322.60476744184</v>
       </c>
       <c r="H62" s="7">
-        <v>-49.995</v>
+        <v>-93448.72004999999</v>
       </c>
     </row>
     <row r="63">
@@ -2688,22 +2686,22 @@
         <v>PF Charge Slab 1</v>
       </c>
       <c r="C63" s="7">
-        <v>-33.33</v>
+        <v>-6229914.67</v>
       </c>
       <c r="D63" s="7">
-        <v>2.35</v>
+        <v>0.0235</v>
       </c>
       <c r="E63" s="7">
-        <v>-78.3255</v>
+        <v>-146402.994745</v>
       </c>
       <c r="F63" s="7">
         <v>0.02</v>
       </c>
       <c r="G63" s="7">
-        <v>-3916.275</v>
+        <v>-7320149.73725</v>
       </c>
       <c r="H63" s="7">
-        <v>-78.3255</v>
+        <v>-146402.994745</v>
       </c>
     </row>
     <row r="64">
@@ -2717,13 +2715,13 @@
         <v>0</v>
       </c>
       <c r="D64" s="7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E64" s="7">
         <v>0</v>
       </c>
       <c r="F64" s="7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G64" s="7">
         <v>0</v>
@@ -2740,22 +2738,22 @@
         <v>Arrear ED</v>
       </c>
       <c r="C65" s="7">
-        <v>14350</v>
+        <v>10924059.54</v>
       </c>
       <c r="D65" s="7">
         <v>0.2</v>
       </c>
       <c r="E65" s="7">
-        <v>2870</v>
+        <v>2184811.908</v>
       </c>
       <c r="F65" s="7">
         <v>1</v>
       </c>
       <c r="G65" s="7">
-        <v>2870</v>
+        <v>2184811.908</v>
       </c>
       <c r="H65" s="7">
-        <v>2870</v>
+        <v>2184811.908</v>
       </c>
     </row>
     <row r="66">
@@ -2769,13 +2767,13 @@
         <v>0</v>
       </c>
       <c r="D66" s="7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E66" s="7">
         <v>0</v>
       </c>
       <c r="F66" s="7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G66" s="7">
         <v>0</v>
@@ -2795,13 +2793,13 @@
         <v>0</v>
       </c>
       <c r="D67" s="7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E67" s="7">
         <v>0</v>
       </c>
       <c r="F67" s="7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G67" s="7">
         <v>0</v>
@@ -2821,13 +2819,13 @@
         <v>0</v>
       </c>
       <c r="D68" s="7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E68" s="7">
         <v>0</v>
       </c>
       <c r="F68" s="7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G68" s="7">
         <v>0</v>
@@ -2853,7 +2851,7 @@
         <v>0</v>
       </c>
       <c r="F69" s="7">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="G69" s="7">
         <v>0</v>
@@ -2892,7 +2890,7 @@
         <v>WEG Billing – Month</v>
       </c>
       <c r="B1" s="1" t="str">
-        <v>2025-07</v>
+        <v>2025-08</v>
       </c>
     </row>
     <row r="2">
@@ -2900,7 +2898,7 @@
         <v>Generated at</v>
       </c>
       <c r="B2" t="str">
-        <v>8/31/2025, 8:55:56 AM</v>
+        <v>9/1/2025, 10:12:12 AM</v>
       </c>
     </row>
     <row r="4">
@@ -2928,7 +2926,7 @@
         <v>A4</v>
       </c>
       <c r="D5" s="2">
-        <v>1000</v>
+        <v>1521462.5</v>
       </c>
       <c r="E5" t="str">
         <v>kWh</v>
@@ -2945,7 +2943,7 @@
         <v>B4</v>
       </c>
       <c r="D6" s="3">
-        <v>5000</v>
+        <v>880925</v>
       </c>
       <c r="E6" t="str">
         <v>₹</v>
@@ -2962,7 +2960,7 @@
         <v>C4</v>
       </c>
       <c r="D7" s="3">
-        <v>8000</v>
+        <v>6390144.6</v>
       </c>
       <c r="E7" t="str">
         <v>₹</v>
@@ -2979,7 +2977,7 @@
         <v>D4</v>
       </c>
       <c r="D8" s="3">
-        <v>200</v>
+        <v>0</v>
       </c>
       <c r="E8" t="str">
         <v>₹</v>
@@ -2996,7 +2994,7 @@
         <v>E4</v>
       </c>
       <c r="D9" s="3">
-        <v>300</v>
+        <v>3727584.35</v>
       </c>
       <c r="E9" t="str">
         <v>₹</v>
@@ -3013,7 +3011,7 @@
         <v>F4</v>
       </c>
       <c r="D10" s="3">
-        <v>100</v>
+        <v>150168.4</v>
       </c>
       <c r="E10" t="str">
         <v>₹</v>
@@ -3030,7 +3028,7 @@
         <v>G4</v>
       </c>
       <c r="D11" s="3">
-        <v>50</v>
+        <v>95852.17</v>
       </c>
       <c r="E11" t="str">
         <v>₹</v>
@@ -3047,7 +3045,7 @@
         <v>H4</v>
       </c>
       <c r="D12" s="3">
-        <v>400</v>
+        <v>430503.75</v>
       </c>
       <c r="E12" t="str">
         <v>₹</v>
@@ -3064,7 +3062,7 @@
         <v>I4</v>
       </c>
       <c r="D13" s="3">
-        <v>600</v>
+        <v>0</v>
       </c>
       <c r="E13" t="str">
         <v>₹</v>
@@ -3081,7 +3079,7 @@
         <v>A9</v>
       </c>
       <c r="D14" s="3">
-        <v>14350</v>
+        <v>11183137.129999999</v>
       </c>
       <c r="E14" t="str">
         <v>₹</v>
@@ -3098,7 +3096,7 @@
         <v>B9</v>
       </c>
       <c r="D15" s="3">
-        <v>2870</v>
+        <v>2236627.426</v>
       </c>
       <c r="E15" t="str">
         <v>₹</v>
@@ -3115,7 +3113,7 @@
         <v>C9</v>
       </c>
       <c r="D16" s="3">
-        <v>17220</v>
+        <v>13419764.555999998</v>
       </c>
       <c r="E16" t="str">
         <v>₹</v>
@@ -3132,7 +3130,7 @@
         <v>D9</v>
       </c>
       <c r="D18" s="3">
-        <v>200</v>
+        <v>16228986.68</v>
       </c>
       <c r="E18" t="str">
         <v>₹</v>
@@ -3149,7 +3147,7 @@
         <v>E9</v>
       </c>
       <c r="D19" s="3">
-        <v>50</v>
+        <v>16222328.84</v>
       </c>
       <c r="E19" t="str">
         <v>₹</v>
@@ -3166,7 +3164,7 @@
         <v>F9</v>
       </c>
       <c r="D20" s="3">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="E20" t="str">
         <v>₹</v>
@@ -3183,7 +3181,7 @@
         <v>G9</v>
       </c>
       <c r="D21" s="3">
-        <v>0</v>
+        <v>5241084.6</v>
       </c>
       <c r="E21" t="str">
         <v>₹</v>
@@ -3200,7 +3198,7 @@
         <v>H9</v>
       </c>
       <c r="D22" s="3">
-        <v>17450</v>
+        <v>24407666.636</v>
       </c>
       <c r="E22" t="str">
         <v>₹</v>
@@ -3217,7 +3215,7 @@
         <v>I9</v>
       </c>
       <c r="D23" s="3">
-        <v>17400</v>
+        <v>8185337.796</v>
       </c>
       <c r="E23" t="str">
         <v>₹</v>
@@ -3234,7 +3232,7 @@
         <v>A31</v>
       </c>
       <c r="D24" s="3">
-        <v>150</v>
+        <v>6657.839999999851</v>
       </c>
       <c r="E24" t="str">
         <v>₹</v>
@@ -3251,7 +3249,7 @@
         <v>B15</v>
       </c>
       <c r="D26" s="4">
-        <v>0.3</v>
+        <v>0.45</v>
       </c>
       <c r="E26" t="str">
         <v>%</v>
@@ -3268,7 +3266,7 @@
         <v>D15</v>
       </c>
       <c r="D27" s="4">
-        <v>0.7</v>
+        <v>0.38</v>
       </c>
       <c r="E27" t="str">
         <v>%</v>
@@ -3285,7 +3283,7 @@
         <v>C16</v>
       </c>
       <c r="D28" s="4">
-        <v>0.02</v>
+        <v>0.0356</v>
       </c>
       <c r="E28" t="str">
         <v>%</v>
@@ -3302,7 +3300,7 @@
         <v>A17</v>
       </c>
       <c r="D29" s="5">
-        <v>1</v>
+        <v>419.961</v>
       </c>
       <c r="E29" t="str">
         <v>MWh</v>
@@ -3319,7 +3317,7 @@
         <v>B17</v>
       </c>
       <c r="D30" s="5">
-        <v>1</v>
+        <v>216.344</v>
       </c>
       <c r="E30" t="str">
         <v>MWh</v>
@@ -3336,7 +3334,7 @@
         <v>C17</v>
       </c>
       <c r="D31" s="5">
-        <v>2</v>
+        <v>513.446</v>
       </c>
       <c r="E31" t="str">
         <v>MWh</v>
@@ -3353,7 +3351,7 @@
         <v>D17</v>
       </c>
       <c r="D32" s="5">
-        <v>1</v>
+        <v>1272.452</v>
       </c>
       <c r="E32" t="str">
         <v>MWh</v>
@@ -3370,7 +3368,7 @@
         <v>E17</v>
       </c>
       <c r="D33" s="5">
-        <v>1</v>
+        <v>446.474</v>
       </c>
       <c r="E33" t="str">
         <v>MWh</v>
@@ -3387,7 +3385,7 @@
         <v>A18</v>
       </c>
       <c r="D34" s="2">
-        <v>588</v>
+        <v>276144</v>
       </c>
       <c r="E34" t="str">
         <v>kWh</v>
@@ -3404,7 +3402,7 @@
         <v>C18</v>
       </c>
       <c r="D35" s="2">
-        <v>2744</v>
+        <v>818102</v>
       </c>
       <c r="E35" t="str">
         <v>kWh</v>
@@ -3421,7 +3419,7 @@
         <v>A19</v>
       </c>
       <c r="D36" s="2">
-        <v>3332</v>
+        <v>1094246</v>
       </c>
       <c r="E36" t="str">
         <v>kWh</v>
@@ -3438,7 +3436,7 @@
         <v>A24</v>
       </c>
       <c r="D38" s="3">
-        <v>500</v>
+        <v>4393406.09</v>
       </c>
       <c r="E38" t="str">
         <v>₹</v>
@@ -3455,7 +3453,7 @@
         <v>B24</v>
       </c>
       <c r="D39" s="3">
-        <v>200</v>
+        <v>878681.22</v>
       </c>
       <c r="E39" t="str">
         <v>₹</v>
@@ -3472,7 +3470,7 @@
         <v>C24</v>
       </c>
       <c r="D40" s="3">
-        <v>100</v>
+        <v>6653</v>
       </c>
       <c r="E40" t="str">
         <v>₹</v>
@@ -3489,7 +3487,7 @@
         <v>D24</v>
       </c>
       <c r="D41" s="3">
-        <v>50</v>
+        <v>3362.44</v>
       </c>
       <c r="E41" t="str">
         <v>₹</v>
@@ -3506,7 +3504,7 @@
         <v>E24</v>
       </c>
       <c r="D42" s="3">
-        <v>25</v>
+        <v>672.48</v>
       </c>
       <c r="E42" t="str">
         <v>₹</v>
@@ -3523,7 +3521,7 @@
         <v>F24</v>
       </c>
       <c r="D43" s="3">
-        <v>25</v>
+        <v>33620.79</v>
       </c>
       <c r="E43" t="str">
         <v>₹</v>
@@ -3540,7 +3538,7 @@
         <v>A26</v>
       </c>
       <c r="D44" s="3">
-        <v>700</v>
+        <v>5272087.31</v>
       </c>
       <c r="E44" t="str">
         <v>₹</v>
@@ -3557,7 +3555,7 @@
         <v>B26</v>
       </c>
       <c r="D45" s="3">
-        <v>100</v>
+        <v>37655.71</v>
       </c>
       <c r="E45" t="str">
         <v>₹</v>
@@ -3574,7 +3572,7 @@
         <v>C26</v>
       </c>
       <c r="D46" s="3">
-        <v>600</v>
+        <v>5234431.6</v>
       </c>
       <c r="E46" t="str">
         <v>₹</v>
@@ -3591,7 +3589,7 @@
         <v>B19</v>
       </c>
       <c r="D47" s="6">
-        <v>0.18007202881152462</v>
+        <v>4.783596741500539</v>
       </c>
       <c r="E47" t="str">
         <v>₹/kWh</v>
@@ -3608,7 +3606,7 @@
         <v>F16</v>
       </c>
       <c r="D48" s="3">
-        <v>105.88235294117648</v>
+        <v>1320961.538584925</v>
       </c>
       <c r="E48" t="str">
         <v>₹</v>
@@ -3625,7 +3623,7 @@
         <v>G16</v>
       </c>
       <c r="D49" s="3">
-        <v>494.11764705882354</v>
+        <v>3913470.0614150744</v>
       </c>
       <c r="E49" t="str">
         <v>₹</v>
@@ -3642,7 +3640,7 @@
         <v>—</v>
       </c>
       <c r="D51" s="3">
-        <v>16700</v>
+        <v>8185337.795999998</v>
       </c>
       <c r="E51" t="str">
         <v>₹</v>
@@ -3691,7 +3689,7 @@
         <v>0</v>
       </c>
       <c r="F54" s="7">
-        <v>750</v>
+        <v>0</v>
       </c>
       <c r="G54" s="7">
         <v>0</v>
@@ -3760,22 +3758,22 @@
         <v>MD Slab 3</v>
       </c>
       <c r="C57" s="7">
-        <v>-421.05</v>
+        <v>1423</v>
       </c>
       <c r="D57" s="7">
         <v>475</v>
       </c>
       <c r="E57" s="7">
-        <v>-199998.75</v>
+        <v>675925</v>
       </c>
       <c r="F57" s="7">
         <v>475</v>
       </c>
       <c r="G57" s="7">
-        <v>-421.05</v>
+        <v>1423</v>
       </c>
       <c r="H57" s="7">
-        <v>-199998.75</v>
+        <v>675925</v>
       </c>
     </row>
     <row r="58">
@@ -3795,7 +3793,7 @@
         <v>0</v>
       </c>
       <c r="F58" s="7">
-        <v>370</v>
+        <v>0</v>
       </c>
       <c r="G58" s="7">
         <v>0</v>
@@ -3812,22 +3810,22 @@
         <v>Energy Charge Slab 1</v>
       </c>
       <c r="C59" s="7">
-        <v>1000</v>
+        <v>1521462.5</v>
       </c>
       <c r="D59" s="7">
         <v>4.2</v>
       </c>
       <c r="E59" s="7">
-        <v>4200</v>
+        <v>6390142.5</v>
       </c>
       <c r="F59" s="7">
         <v>4.2</v>
       </c>
       <c r="G59" s="7">
-        <v>1000</v>
+        <v>1521462.5</v>
       </c>
       <c r="H59" s="7">
-        <v>4200</v>
+        <v>6390142.5</v>
       </c>
     </row>
     <row r="60">
@@ -3838,22 +3836,22 @@
         <v>FCA</v>
       </c>
       <c r="C60" s="7">
-        <v>1000</v>
+        <v>1521462.5</v>
       </c>
       <c r="D60" s="7">
         <v>2.45</v>
       </c>
       <c r="E60" s="7">
-        <v>2450</v>
+        <v>3727583.1250000005</v>
       </c>
       <c r="F60" s="7">
         <v>1.81</v>
       </c>
       <c r="G60" s="7">
-        <v>1353.5911602209944</v>
+        <v>2059438.190607735</v>
       </c>
       <c r="H60" s="7">
-        <v>2450</v>
+        <v>3727583.1250000005</v>
       </c>
     </row>
     <row r="61">
@@ -3864,22 +3862,22 @@
         <v>TOD Peak</v>
       </c>
       <c r="C61" s="7">
-        <v>470.59</v>
+        <v>506475</v>
       </c>
       <c r="D61" s="7">
         <v>0.85</v>
       </c>
       <c r="E61" s="7">
-        <v>400.00149999999996</v>
+        <v>430503.75</v>
       </c>
       <c r="F61" s="7">
         <v>0.85</v>
       </c>
       <c r="G61" s="7">
-        <v>470.59</v>
+        <v>506475</v>
       </c>
       <c r="H61" s="7">
-        <v>400.00149999999996</v>
+        <v>430503.75</v>
       </c>
     </row>
     <row r="62">
@@ -3890,22 +3888,22 @@
         <v>TOD Night Rebate</v>
       </c>
       <c r="C62" s="7">
-        <v>-33.33</v>
+        <v>-6390144.67</v>
       </c>
       <c r="D62" s="7">
-        <v>1.5</v>
+        <v>0.015</v>
       </c>
       <c r="E62" s="7">
-        <v>-49.995</v>
+        <v>-95852.17005</v>
       </c>
       <c r="F62" s="7">
         <v>0.43</v>
       </c>
       <c r="G62" s="7">
-        <v>-116.26744186046511</v>
+        <v>-222912.02337209304</v>
       </c>
       <c r="H62" s="7">
-        <v>-49.995</v>
+        <v>-95852.17005</v>
       </c>
     </row>
     <row r="63">
@@ -3916,22 +3914,22 @@
         <v>PF Charge Slab 1</v>
       </c>
       <c r="C63" s="7">
-        <v>-33.33</v>
+        <v>-6390144.67</v>
       </c>
       <c r="D63" s="7">
-        <v>2.35</v>
+        <v>0.0235</v>
       </c>
       <c r="E63" s="7">
-        <v>-78.3255</v>
+        <v>-150168.399745</v>
       </c>
       <c r="F63" s="7">
         <v>0.02</v>
       </c>
       <c r="G63" s="7">
-        <v>-3916.275</v>
+        <v>-7508419.98725</v>
       </c>
       <c r="H63" s="7">
-        <v>-78.3255</v>
+        <v>-150168.399745</v>
       </c>
     </row>
     <row r="64">
@@ -3945,13 +3943,13 @@
         <v>0</v>
       </c>
       <c r="D64" s="7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E64" s="7">
         <v>0</v>
       </c>
       <c r="F64" s="7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G64" s="7">
         <v>0</v>
@@ -3968,22 +3966,22 @@
         <v>Arrear ED</v>
       </c>
       <c r="C65" s="7">
-        <v>14350</v>
+        <v>11183137.13</v>
       </c>
       <c r="D65" s="7">
         <v>0.2</v>
       </c>
       <c r="E65" s="7">
-        <v>2870</v>
+        <v>2236627.4260000004</v>
       </c>
       <c r="F65" s="7">
         <v>1</v>
       </c>
       <c r="G65" s="7">
-        <v>2870</v>
+        <v>2236627.4260000004</v>
       </c>
       <c r="H65" s="7">
-        <v>2870</v>
+        <v>2236627.4260000004</v>
       </c>
     </row>
     <row r="66">
@@ -3997,13 +3995,13 @@
         <v>0</v>
       </c>
       <c r="D66" s="7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E66" s="7">
         <v>0</v>
       </c>
       <c r="F66" s="7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G66" s="7">
         <v>0</v>
@@ -4023,13 +4021,13 @@
         <v>0</v>
       </c>
       <c r="D67" s="7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E67" s="7">
         <v>0</v>
       </c>
       <c r="F67" s="7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G67" s="7">
         <v>0</v>
@@ -4049,13 +4047,13 @@
         <v>0</v>
       </c>
       <c r="D68" s="7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E68" s="7">
         <v>0</v>
       </c>
       <c r="F68" s="7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G68" s="7">
         <v>0</v>
@@ -4081,1235 +4079,7 @@
         <v>0</v>
       </c>
       <c r="F69" s="7">
-        <v>-1</v>
-      </c>
-      <c r="G69" s="7">
-        <v>0</v>
-      </c>
-      <c r="H69" s="7">
-        <v>0</v>
-      </c>
-    </row>
-  </sheetData>
-  <autoFilter ref="A4:E51"/>
-  <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:H69"/>
-  </ignoredErrors>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H69"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <cols>
-    <col min="1" max="1" width="18.83203125" customWidth="1"/>
-    <col min="2" max="2" width="32.83203125" customWidth="1"/>
-    <col min="3" max="3" width="8.83203125" customWidth="1"/>
-    <col min="4" max="4" width="16.83203125" customWidth="1"/>
-    <col min="5" max="5" width="36.83203125" customWidth="1"/>
-    <col min="6" max="6" width="14.83203125" customWidth="1"/>
-    <col min="7" max="7" width="12.83203125" customWidth="1"/>
-    <col min="8" max="8" width="14.83203125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="str">
-        <v>WEG Billing – Month</v>
-      </c>
-      <c r="B1" s="1" t="str">
-        <v>2025-08</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="str">
-        <v>Generated at</v>
-      </c>
-      <c r="B2" t="str">
-        <v>8/31/2025, 8:57:33 AM</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="str">
-        <v>SECTION</v>
-      </c>
-      <c r="B4" t="str">
-        <v>FIELD</v>
-      </c>
-      <c r="C4" t="str">
-        <v>CELL</v>
-      </c>
-      <c r="E4" t="str">
-        <v>UNITS/NOTES</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="str">
-        <v>HT Bill</v>
-      </c>
-      <c r="B5" t="str">
-        <v>Monthly Consumption</v>
-      </c>
-      <c r="C5" t="str">
-        <v>A4</v>
-      </c>
-      <c r="D5" s="2">
-        <v>1000</v>
-      </c>
-      <c r="E5" t="str">
-        <v>kWh</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="str">
-        <v>HT Bill</v>
-      </c>
-      <c r="B6" t="str">
-        <v>Demand Charges</v>
-      </c>
-      <c r="C6" t="str">
-        <v>B4</v>
-      </c>
-      <c r="D6" s="3">
-        <v>5000</v>
-      </c>
-      <c r="E6" t="str">
-        <v>₹</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="str">
-        <v>HT Bill</v>
-      </c>
-      <c r="B7" t="str">
-        <v>Energy Charges</v>
-      </c>
-      <c r="C7" t="str">
-        <v>C4</v>
-      </c>
-      <c r="D7" s="3">
-        <v>8000</v>
-      </c>
-      <c r="E7" t="str">
-        <v>₹</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="str">
-        <v>HT Bill</v>
-      </c>
-      <c r="B8" t="str">
-        <v>Night Rebate</v>
-      </c>
-      <c r="C8" t="str">
-        <v>D4</v>
-      </c>
-      <c r="D8" s="3">
-        <v>200</v>
-      </c>
-      <c r="E8" t="str">
-        <v>₹</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="str">
-        <v>HT Bill</v>
-      </c>
-      <c r="B9" t="str">
-        <v>Fuel Charge</v>
-      </c>
-      <c r="C9" t="str">
-        <v>E4</v>
-      </c>
-      <c r="D9" s="3">
-        <v>300</v>
-      </c>
-      <c r="E9" t="str">
-        <v>₹</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="str">
-        <v>HT Bill</v>
-      </c>
-      <c r="B10" t="str">
-        <v>PF Rebate</v>
-      </c>
-      <c r="C10" t="str">
-        <v>F4</v>
-      </c>
-      <c r="D10" s="3">
-        <v>100</v>
-      </c>
-      <c r="E10" t="str">
-        <v>₹</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="str">
-        <v>HT Bill</v>
-      </c>
-      <c r="B11" t="str">
-        <v>EHV Rebate</v>
-      </c>
-      <c r="C11" t="str">
-        <v>G4</v>
-      </c>
-      <c r="D11" s="3">
-        <v>50</v>
-      </c>
-      <c r="E11" t="str">
-        <v>₹</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="str">
-        <v>HT Bill</v>
-      </c>
-      <c r="B12" t="str">
-        <v>TOU</v>
-      </c>
-      <c r="C12" t="str">
-        <v>H4</v>
-      </c>
-      <c r="D12" s="3">
-        <v>400</v>
-      </c>
-      <c r="E12" t="str">
-        <v>₹</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="str">
-        <v>HT Bill</v>
-      </c>
-      <c r="B13" t="str">
-        <v>GT Charges</v>
-      </c>
-      <c r="C13" t="str">
-        <v>I4</v>
-      </c>
-      <c r="D13" s="3">
-        <v>600</v>
-      </c>
-      <c r="E13" t="str">
-        <v>₹</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="str">
-        <v>HT Bill (calc)</v>
-      </c>
-      <c r="B14" t="str">
-        <v>Total Consumption Charge</v>
-      </c>
-      <c r="C14" t="str">
-        <v>A9</v>
-      </c>
-      <c r="D14" s="3">
-        <v>14350</v>
-      </c>
-      <c r="E14" t="str">
-        <v>₹</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="str">
-        <v>HT Bill (calc)</v>
-      </c>
-      <c r="B15" t="str">
-        <v>ED @ 20%</v>
-      </c>
-      <c r="C15" t="str">
-        <v>B9</v>
-      </c>
-      <c r="D15" s="3">
-        <v>2870</v>
-      </c>
-      <c r="E15" t="str">
-        <v>₹</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="str">
-        <v>HT Bill (calc)</v>
-      </c>
-      <c r="B16" t="str">
-        <v>Current Month Bill</v>
-      </c>
-      <c r="C16" t="str">
-        <v>C9</v>
-      </c>
-      <c r="D16" s="3">
-        <v>17220</v>
-      </c>
-      <c r="E16" t="str">
-        <v>₹</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="str">
-        <v>Adjust</v>
-      </c>
-      <c r="B18" t="str">
-        <v>Outstanding Arrears</v>
-      </c>
-      <c r="C18" t="str">
-        <v>D9</v>
-      </c>
-      <c r="D18" s="3">
-        <v>200</v>
-      </c>
-      <c r="E18" t="str">
-        <v>₹</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="str">
-        <v>Adjust</v>
-      </c>
-      <c r="B19" t="str">
-        <v>Freeze Amount</v>
-      </c>
-      <c r="C19" t="str">
-        <v>E9</v>
-      </c>
-      <c r="D19" s="3">
-        <v>50</v>
-      </c>
-      <c r="E19" t="str">
-        <v>₹</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="str">
-        <v>Adjust</v>
-      </c>
-      <c r="B20" t="str">
-        <v>Delayed Payment Charges</v>
-      </c>
-      <c r="C20" t="str">
-        <v>F9</v>
-      </c>
-      <c r="D20" s="3">
-        <v>30</v>
-      </c>
-      <c r="E20" t="str">
-        <v>₹</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="str">
-        <v>Adjust</v>
-      </c>
-      <c r="B21" t="str">
-        <v>Advance Payment / Adjust.</v>
-      </c>
-      <c r="C21" t="str">
-        <v>G9</v>
-      </c>
-      <c r="D21" s="3">
-        <v>0</v>
-      </c>
-      <c r="E21" t="str">
-        <v>₹</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="str">
-        <v>Adjust (calc)</v>
-      </c>
-      <c r="B22" t="str">
-        <v>Net Payable</v>
-      </c>
-      <c r="C22" t="str">
-        <v>H9</v>
-      </c>
-      <c r="D22" s="3">
-        <v>17450</v>
-      </c>
-      <c r="E22" t="str">
-        <v>₹</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" t="str">
-        <v>Adjust (calc)</v>
-      </c>
-      <c r="B23" t="str">
-        <v>Actual Amount to be Paid</v>
-      </c>
-      <c r="C23" t="str">
-        <v>I9</v>
-      </c>
-      <c r="D23" s="3">
-        <v>17400</v>
-      </c>
-      <c r="E23" t="str">
-        <v>₹</v>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" t="str">
-        <v>Adjust (calc)</v>
-      </c>
-      <c r="B24" t="str">
-        <v>Balance Pending from Previous Month</v>
-      </c>
-      <c r="C24" t="str">
-        <v>A31</v>
-      </c>
-      <c r="D24" s="3">
-        <v>150</v>
-      </c>
-      <c r="E24" t="str">
-        <v>₹</v>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" t="str">
-        <v>WEG</v>
-      </c>
-      <c r="B26" t="str">
-        <v>Share Bitlavadia (%)</v>
-      </c>
-      <c r="C26" t="str">
-        <v>B15</v>
-      </c>
-      <c r="D26" s="4">
-        <v>0.3</v>
-      </c>
-      <c r="E26" t="str">
-        <v>%</v>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" t="str">
-        <v>WEG</v>
-      </c>
-      <c r="B27" t="str">
-        <v>Share Nanisindhodi (%)</v>
-      </c>
-      <c r="C27" t="str">
-        <v>D15</v>
-      </c>
-      <c r="D27" s="4">
-        <v>0.7</v>
-      </c>
-      <c r="E27" t="str">
-        <v>%</v>
-      </c>
-    </row>
-    <row r="28">
-      <c r="A28" t="str">
-        <v>WEG</v>
-      </c>
-      <c r="B28" t="str">
-        <v>Transmission Loss (%)</v>
-      </c>
-      <c r="C28" t="str">
-        <v>C16</v>
-      </c>
-      <c r="D28" s="4">
-        <v>0.02</v>
-      </c>
-      <c r="E28" t="str">
-        <v>%</v>
-      </c>
-    </row>
-    <row r="29">
-      <c r="A29" t="str">
-        <v>WEG</v>
-      </c>
-      <c r="B29" t="str">
-        <v>Bitlavadia MWh #1</v>
-      </c>
-      <c r="C29" t="str">
-        <v>A17</v>
-      </c>
-      <c r="D29" s="5">
-        <v>1</v>
-      </c>
-      <c r="E29" t="str">
-        <v>MWh</v>
-      </c>
-    </row>
-    <row r="30">
-      <c r="A30" t="str">
-        <v>WEG</v>
-      </c>
-      <c r="B30" t="str">
-        <v>Bitlavadia MWh #2</v>
-      </c>
-      <c r="C30" t="str">
-        <v>B17</v>
-      </c>
-      <c r="D30" s="5">
-        <v>1</v>
-      </c>
-      <c r="E30" t="str">
-        <v>MWh</v>
-      </c>
-    </row>
-    <row r="31">
-      <c r="A31" t="str">
-        <v>WEG</v>
-      </c>
-      <c r="B31" t="str">
-        <v>Nanisindhodi MWh #1</v>
-      </c>
-      <c r="C31" t="str">
-        <v>C17</v>
-      </c>
-      <c r="D31" s="5">
-        <v>2</v>
-      </c>
-      <c r="E31" t="str">
-        <v>MWh</v>
-      </c>
-    </row>
-    <row r="32">
-      <c r="A32" t="str">
-        <v>WEG</v>
-      </c>
-      <c r="B32" t="str">
-        <v>Nanisindhodi MWh #2</v>
-      </c>
-      <c r="C32" t="str">
-        <v>D17</v>
-      </c>
-      <c r="D32" s="5">
-        <v>1</v>
-      </c>
-      <c r="E32" t="str">
-        <v>MWh</v>
-      </c>
-    </row>
-    <row r="33">
-      <c r="A33" t="str">
-        <v>WEG</v>
-      </c>
-      <c r="B33" t="str">
-        <v>Nanisindhodi MWh #3</v>
-      </c>
-      <c r="C33" t="str">
-        <v>E17</v>
-      </c>
-      <c r="D33" s="5">
-        <v>1</v>
-      </c>
-      <c r="E33" t="str">
-        <v>MWh</v>
-      </c>
-    </row>
-    <row r="34">
-      <c r="A34" t="str">
-        <v>WEG (calc)</v>
-      </c>
-      <c r="B34" t="str">
-        <v>Bitlavadia Share (kWh)</v>
-      </c>
-      <c r="C34" t="str">
-        <v>A18</v>
-      </c>
-      <c r="D34" s="2">
-        <v>588</v>
-      </c>
-      <c r="E34" t="str">
-        <v>kWh</v>
-      </c>
-    </row>
-    <row r="35">
-      <c r="A35" t="str">
-        <v>WEG (calc)</v>
-      </c>
-      <c r="B35" t="str">
-        <v>Nanisindhodi Share (kWh)</v>
-      </c>
-      <c r="C35" t="str">
-        <v>C18</v>
-      </c>
-      <c r="D35" s="2">
-        <v>2744</v>
-      </c>
-      <c r="E35" t="str">
-        <v>kWh</v>
-      </c>
-    </row>
-    <row r="36">
-      <c r="A36" t="str">
-        <v>WEG (calc)</v>
-      </c>
-      <c r="B36" t="str">
-        <v>Total Allocated (kWh)</v>
-      </c>
-      <c r="C36" t="str">
-        <v>A19</v>
-      </c>
-      <c r="D36" s="2">
-        <v>3332</v>
-      </c>
-      <c r="E36" t="str">
-        <v>kWh</v>
-      </c>
-    </row>
-    <row r="38">
-      <c r="A38" t="str">
-        <v>Wind Credits</v>
-      </c>
-      <c r="B38" t="str">
-        <v>Credit Board Charges</v>
-      </c>
-      <c r="C38" t="str">
-        <v>A24</v>
-      </c>
-      <c r="D38" s="3">
-        <v>500</v>
-      </c>
-      <c r="E38" t="str">
-        <v>₹</v>
-      </c>
-    </row>
-    <row r="39">
-      <c r="A39" t="str">
-        <v>Wind Credits</v>
-      </c>
-      <c r="B39" t="str">
-        <v>Credit ED Charges</v>
-      </c>
-      <c r="C39" t="str">
-        <v>B24</v>
-      </c>
-      <c r="D39" s="3">
-        <v>200</v>
-      </c>
-      <c r="E39" t="str">
-        <v>₹</v>
-      </c>
-    </row>
-    <row r="40">
-      <c r="A40" t="str">
-        <v>Wind Credits</v>
-      </c>
-      <c r="B40" t="str">
-        <v>Credit TDS</v>
-      </c>
-      <c r="C40" t="str">
-        <v>C24</v>
-      </c>
-      <c r="D40" s="3">
-        <v>100</v>
-      </c>
-      <c r="E40" t="str">
-        <v>₹</v>
-      </c>
-    </row>
-    <row r="41">
-      <c r="A41" t="str">
-        <v>Wind Debits</v>
-      </c>
-      <c r="B41" t="str">
-        <v>Debit Board Charges</v>
-      </c>
-      <c r="C41" t="str">
-        <v>D24</v>
-      </c>
-      <c r="D41" s="3">
-        <v>50</v>
-      </c>
-      <c r="E41" t="str">
-        <v>₹</v>
-      </c>
-    </row>
-    <row r="42">
-      <c r="A42" t="str">
-        <v>Wind Debits</v>
-      </c>
-      <c r="B42" t="str">
-        <v>Debit Electricity Duty</v>
-      </c>
-      <c r="C42" t="str">
-        <v>E24</v>
-      </c>
-      <c r="D42" s="3">
-        <v>25</v>
-      </c>
-      <c r="E42" t="str">
-        <v>₹</v>
-      </c>
-    </row>
-    <row r="43">
-      <c r="A43" t="str">
-        <v>Wind Debits</v>
-      </c>
-      <c r="B43" t="str">
-        <v>Debit Wheeling Charges</v>
-      </c>
-      <c r="C43" t="str">
-        <v>F24</v>
-      </c>
-      <c r="D43" s="3">
-        <v>25</v>
-      </c>
-      <c r="E43" t="str">
-        <v>₹</v>
-      </c>
-    </row>
-    <row r="44">
-      <c r="A44" t="str">
-        <v>Wind (calc)</v>
-      </c>
-      <c r="B44" t="str">
-        <v>Total Credit</v>
-      </c>
-      <c r="C44" t="str">
-        <v>A26</v>
-      </c>
-      <c r="D44" s="3">
-        <v>700</v>
-      </c>
-      <c r="E44" t="str">
-        <v>₹</v>
-      </c>
-    </row>
-    <row r="45">
-      <c r="A45" t="str">
-        <v>Wind (calc)</v>
-      </c>
-      <c r="B45" t="str">
-        <v>Total Debit</v>
-      </c>
-      <c r="C45" t="str">
-        <v>B26</v>
-      </c>
-      <c r="D45" s="3">
-        <v>100</v>
-      </c>
-      <c r="E45" t="str">
-        <v>₹</v>
-      </c>
-    </row>
-    <row r="46">
-      <c r="A46" t="str">
-        <v>Wind (calc)</v>
-      </c>
-      <c r="B46" t="str">
-        <v>Net Wind Credit</v>
-      </c>
-      <c r="C46" t="str">
-        <v>C26</v>
-      </c>
-      <c r="D46" s="3">
-        <v>600</v>
-      </c>
-      <c r="E46" t="str">
-        <v>₹</v>
-      </c>
-    </row>
-    <row r="47">
-      <c r="A47" t="str">
-        <v>Wind (calc)</v>
-      </c>
-      <c r="B47" t="str">
-        <v>Wind Rate (₹/kWh)</v>
-      </c>
-      <c r="C47" t="str">
-        <v>B19</v>
-      </c>
-      <c r="D47" s="6">
-        <v>0.18007202881152462</v>
-      </c>
-      <c r="E47" t="str">
-        <v>₹/kWh</v>
-      </c>
-    </row>
-    <row r="48">
-      <c r="A48" t="str">
-        <v>Wind (calc)</v>
-      </c>
-      <c r="B48" t="str">
-        <v>Share 4.5 MW (₹)</v>
-      </c>
-      <c r="C48" t="str">
-        <v>F16</v>
-      </c>
-      <c r="D48" s="3">
-        <v>105.88235294117648</v>
-      </c>
-      <c r="E48" t="str">
-        <v>₹</v>
-      </c>
-    </row>
-    <row r="49">
-      <c r="A49" t="str">
-        <v>Wind (calc)</v>
-      </c>
-      <c r="B49" t="str">
-        <v>Share 14.7 MW (₹)</v>
-      </c>
-      <c r="C49" t="str">
-        <v>G16</v>
-      </c>
-      <c r="D49" s="3">
-        <v>494.11764705882354</v>
-      </c>
-      <c r="E49" t="str">
-        <v>₹</v>
-      </c>
-    </row>
-    <row r="51">
-      <c r="A51" t="str">
-        <v>FINAL</v>
-      </c>
-      <c r="B51" t="str">
-        <v>Final Bill for IOM</v>
-      </c>
-      <c r="C51" t="str">
-        <v>—</v>
-      </c>
-      <c r="D51" s="3">
-        <v>16700</v>
-      </c>
-      <c r="E51" t="str">
-        <v>₹</v>
-      </c>
-    </row>
-    <row r="53">
-      <c r="A53" t="str">
-        <v>Service Code</v>
-      </c>
-      <c r="B53" t="str">
-        <v>Service Name</v>
-      </c>
-      <c r="C53" t="str">
-        <v>Qty (B)</v>
-      </c>
-      <c r="D53" t="str">
-        <v>Tariff (C)</v>
-      </c>
-      <c r="E53" t="str">
-        <v>Amt (D)</v>
-      </c>
-      <c r="F53" t="str">
-        <v>Contract Rate (E)</v>
-      </c>
-      <c r="G53" t="str">
-        <v>Unit Adj (F)</v>
-      </c>
-      <c r="H53" t="str">
-        <v>Amount SES (G)</v>
-      </c>
-    </row>
-    <row r="54">
-      <c r="A54" t="str">
-        <v>FIXED_METER_RENT</v>
-      </c>
-      <c r="B54" t="str">
-        <v>Fixed Meter Rent</v>
-      </c>
-      <c r="C54" s="7">
-        <v>0</v>
-      </c>
-      <c r="D54" s="7">
-        <v>0</v>
-      </c>
-      <c r="E54" s="7">
-        <v>0</v>
-      </c>
-      <c r="F54" s="7">
-        <v>750</v>
-      </c>
-      <c r="G54" s="7">
-        <v>0</v>
-      </c>
-      <c r="H54" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="55">
-      <c r="A55" t="str">
-        <v>MD_SLAB1</v>
-      </c>
-      <c r="B55" t="str">
-        <v>MD Slab 1</v>
-      </c>
-      <c r="C55" s="7">
-        <v>500</v>
-      </c>
-      <c r="D55" s="7">
-        <v>150</v>
-      </c>
-      <c r="E55" s="7">
-        <v>75000</v>
-      </c>
-      <c r="F55" s="7">
-        <v>150</v>
-      </c>
-      <c r="G55" s="7">
-        <v>500</v>
-      </c>
-      <c r="H55" s="7">
-        <v>75000</v>
-      </c>
-    </row>
-    <row r="56">
-      <c r="A56" t="str">
-        <v>MD_SLAB2</v>
-      </c>
-      <c r="B56" t="str">
-        <v>MD Slab 2</v>
-      </c>
-      <c r="C56" s="7">
-        <v>500</v>
-      </c>
-      <c r="D56" s="7">
-        <v>260</v>
-      </c>
-      <c r="E56" s="7">
-        <v>130000</v>
-      </c>
-      <c r="F56" s="7">
-        <v>260</v>
-      </c>
-      <c r="G56" s="7">
-        <v>500</v>
-      </c>
-      <c r="H56" s="7">
-        <v>130000</v>
-      </c>
-    </row>
-    <row r="57">
-      <c r="A57" t="str">
-        <v>MD_SLAB3</v>
-      </c>
-      <c r="B57" t="str">
-        <v>MD Slab 3</v>
-      </c>
-      <c r="C57" s="7">
-        <v>-421.05</v>
-      </c>
-      <c r="D57" s="7">
-        <v>475</v>
-      </c>
-      <c r="E57" s="7">
-        <v>-199998.75</v>
-      </c>
-      <c r="F57" s="7">
-        <v>475</v>
-      </c>
-      <c r="G57" s="7">
-        <v>-421.05</v>
-      </c>
-      <c r="H57" s="7">
-        <v>-199998.75</v>
-      </c>
-    </row>
-    <row r="58">
-      <c r="A58" t="str">
-        <v>PENAL_ABOVE_CD</v>
-      </c>
-      <c r="B58" t="str">
-        <v>Penal Above CD</v>
-      </c>
-      <c r="C58" s="7">
-        <v>0</v>
-      </c>
-      <c r="D58" s="7">
-        <v>0</v>
-      </c>
-      <c r="E58" s="7">
-        <v>0</v>
-      </c>
-      <c r="F58" s="7">
-        <v>370</v>
-      </c>
-      <c r="G58" s="7">
-        <v>0</v>
-      </c>
-      <c r="H58" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="59">
-      <c r="A59" t="str">
-        <v>EC_SLAB1</v>
-      </c>
-      <c r="B59" t="str">
-        <v>Energy Charge Slab 1</v>
-      </c>
-      <c r="C59" s="7">
-        <v>1000</v>
-      </c>
-      <c r="D59" s="7">
-        <v>4.2</v>
-      </c>
-      <c r="E59" s="7">
-        <v>4200</v>
-      </c>
-      <c r="F59" s="7">
-        <v>4.2</v>
-      </c>
-      <c r="G59" s="7">
-        <v>1000</v>
-      </c>
-      <c r="H59" s="7">
-        <v>4200</v>
-      </c>
-    </row>
-    <row r="60">
-      <c r="A60" t="str">
-        <v>FCA</v>
-      </c>
-      <c r="B60" t="str">
-        <v>FCA</v>
-      </c>
-      <c r="C60" s="7">
-        <v>1000</v>
-      </c>
-      <c r="D60" s="7">
-        <v>2.45</v>
-      </c>
-      <c r="E60" s="7">
-        <v>2450</v>
-      </c>
-      <c r="F60" s="7">
-        <v>1.81</v>
-      </c>
-      <c r="G60" s="7">
-        <v>1353.5911602209944</v>
-      </c>
-      <c r="H60" s="7">
-        <v>2450</v>
-      </c>
-    </row>
-    <row r="61">
-      <c r="A61" t="str">
-        <v>TOD_PEAK</v>
-      </c>
-      <c r="B61" t="str">
-        <v>TOD Peak</v>
-      </c>
-      <c r="C61" s="7">
-        <v>470.59</v>
-      </c>
-      <c r="D61" s="7">
-        <v>0.85</v>
-      </c>
-      <c r="E61" s="7">
-        <v>400.00149999999996</v>
-      </c>
-      <c r="F61" s="7">
-        <v>0.85</v>
-      </c>
-      <c r="G61" s="7">
-        <v>470.59</v>
-      </c>
-      <c r="H61" s="7">
-        <v>400.00149999999996</v>
-      </c>
-    </row>
-    <row r="62">
-      <c r="A62" t="str">
-        <v>TOD_NIGHT_REBATE</v>
-      </c>
-      <c r="B62" t="str">
-        <v>TOD Night Rebate</v>
-      </c>
-      <c r="C62" s="7">
-        <v>-33.33</v>
-      </c>
-      <c r="D62" s="7">
-        <v>1.5</v>
-      </c>
-      <c r="E62" s="7">
-        <v>-49.995</v>
-      </c>
-      <c r="F62" s="7">
-        <v>0.43</v>
-      </c>
-      <c r="G62" s="7">
-        <v>-116.26744186046511</v>
-      </c>
-      <c r="H62" s="7">
-        <v>-49.995</v>
-      </c>
-    </row>
-    <row r="63">
-      <c r="A63" t="str">
-        <v>PF_CHARGE_SLAB1</v>
-      </c>
-      <c r="B63" t="str">
-        <v>PF Charge Slab 1</v>
-      </c>
-      <c r="C63" s="7">
-        <v>-33.33</v>
-      </c>
-      <c r="D63" s="7">
-        <v>2.35</v>
-      </c>
-      <c r="E63" s="7">
-        <v>-78.3255</v>
-      </c>
-      <c r="F63" s="7">
-        <v>0.02</v>
-      </c>
-      <c r="G63" s="7">
-        <v>-3916.275</v>
-      </c>
-      <c r="H63" s="7">
-        <v>-78.3255</v>
-      </c>
-    </row>
-    <row r="64">
-      <c r="A64" t="str">
-        <v>ARREAR_FCA</v>
-      </c>
-      <c r="B64" t="str">
-        <v>Arrear FCA</v>
-      </c>
-      <c r="C64" s="7">
-        <v>0</v>
-      </c>
-      <c r="D64" s="7">
-        <v>1</v>
-      </c>
-      <c r="E64" s="7">
-        <v>0</v>
-      </c>
-      <c r="F64" s="7">
-        <v>1</v>
-      </c>
-      <c r="G64" s="7">
-        <v>0</v>
-      </c>
-      <c r="H64" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="65">
-      <c r="A65" t="str">
-        <v>ARREAR_ED</v>
-      </c>
-      <c r="B65" t="str">
-        <v>Arrear ED</v>
-      </c>
-      <c r="C65" s="7">
-        <v>14350</v>
-      </c>
-      <c r="D65" s="7">
-        <v>0.2</v>
-      </c>
-      <c r="E65" s="7">
-        <v>2870</v>
-      </c>
-      <c r="F65" s="7">
-        <v>1</v>
-      </c>
-      <c r="G65" s="7">
-        <v>2870</v>
-      </c>
-      <c r="H65" s="7">
-        <v>2870</v>
-      </c>
-    </row>
-    <row r="66">
-      <c r="A66" t="str">
-        <v>ARREAR_CESS</v>
-      </c>
-      <c r="B66" t="str">
-        <v>Arrear Cess</v>
-      </c>
-      <c r="C66" s="7">
-        <v>0</v>
-      </c>
-      <c r="D66" s="7">
-        <v>1</v>
-      </c>
-      <c r="E66" s="7">
-        <v>0</v>
-      </c>
-      <c r="F66" s="7">
-        <v>1</v>
-      </c>
-      <c r="G66" s="7">
-        <v>0</v>
-      </c>
-      <c r="H66" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="67">
-      <c r="A67" t="str">
-        <v>ARREAR_PF</v>
-      </c>
-      <c r="B67" t="str">
-        <v>Arrear PF</v>
-      </c>
-      <c r="C67" s="7">
-        <v>0</v>
-      </c>
-      <c r="D67" s="7">
-        <v>1</v>
-      </c>
-      <c r="E67" s="7">
-        <v>0</v>
-      </c>
-      <c r="F67" s="7">
-        <v>1</v>
-      </c>
-      <c r="G67" s="7">
-        <v>0</v>
-      </c>
-      <c r="H67" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="68">
-      <c r="A68" t="str">
-        <v>ARREAR_ENERGY</v>
-      </c>
-      <c r="B68" t="str">
-        <v>Arrear Energy</v>
-      </c>
-      <c r="C68" s="7">
-        <v>0</v>
-      </c>
-      <c r="D68" s="7">
-        <v>1</v>
-      </c>
-      <c r="E68" s="7">
-        <v>0</v>
-      </c>
-      <c r="F68" s="7">
-        <v>1</v>
-      </c>
-      <c r="G68" s="7">
-        <v>0</v>
-      </c>
-      <c r="H68" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="69">
-      <c r="A69" t="str">
-        <v>WIND_ENERGY_CREDIT</v>
-      </c>
-      <c r="B69" t="str">
-        <v>Wind Energy Credit</v>
-      </c>
-      <c r="C69" s="7">
-        <v>0</v>
-      </c>
-      <c r="D69" s="7">
-        <v>0</v>
-      </c>
-      <c r="E69" s="7">
-        <v>0</v>
-      </c>
-      <c r="F69" s="7">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="G69" s="7">
         <v>0</v>

</xml_diff>